<commit_message>
Fine esperienza, dobbiamo solo riprendere Brewster (riflesso) e Bragg
</commit_message>
<xml_diff>
--- a/Microonde/dati_bragg.xlsx
+++ b/Microonde/dati_bragg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ALL\Stefano\Bicocca\secondo_anno\lab2\Laboratorio_2\Microonde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDAD721-3133-4DA8-BDC2-305C5CDDD90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332ECECC-657D-4C7A-9030-D36459159166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,7 +351,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A2" sqref="A2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Un piccolo inizio dell'analisi
</commit_message>
<xml_diff>
--- a/Microonde/dati_bragg.xlsx
+++ b/Microonde/dati_bragg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ALL\Stefano\Bicocca\secondo_anno\lab2\Laboratorio_2\Microonde\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesco\Desktop\Desktop Files\Uni\ANNO2\Laboratorio_2\Microonde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06BC48D-88CF-49BB-B56D-B1EC8BB988DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B15C684-EB09-4C6F-81D9-DA45968E62B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -356,19 +356,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -382,7 +380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>90</v>
       </c>
@@ -402,7 +400,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>92</v>
       </c>
@@ -422,7 +420,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>94</v>
       </c>
@@ -442,7 +440,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>96</v>
       </c>
@@ -462,7 +460,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>98</v>
       </c>
@@ -482,7 +480,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>100</v>
       </c>
@@ -502,7 +500,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>102</v>
       </c>
@@ -522,7 +520,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>104</v>
       </c>
@@ -542,7 +540,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>106</v>
       </c>
@@ -556,7 +554,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>108</v>
       </c>
@@ -570,7 +568,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>110</v>
       </c>
@@ -584,7 +582,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>112</v>
       </c>
@@ -598,7 +596,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>114</v>
       </c>
@@ -612,7 +610,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>116</v>
       </c>
@@ -626,7 +624,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>118</v>
       </c>
@@ -640,7 +638,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>120</v>
       </c>
@@ -654,7 +652,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>122</v>
       </c>
@@ -668,7 +666,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>124</v>
       </c>
@@ -682,7 +680,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>126</v>
       </c>
@@ -696,7 +694,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>128</v>
       </c>
@@ -710,7 +708,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>130</v>
       </c>
@@ -724,7 +722,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>132</v>
       </c>
@@ -732,7 +730,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>134</v>
       </c>
@@ -740,7 +738,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>136</v>
       </c>
@@ -748,7 +746,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>138</v>
       </c>
@@ -756,7 +754,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>140</v>
       </c>
@@ -764,7 +762,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>142</v>
       </c>
@@ -772,7 +770,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>146</v>
       </c>
@@ -780,7 +778,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>148</v>
       </c>
@@ -788,7 +786,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>150</v>
       </c>
@@ -796,7 +794,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>152</v>
       </c>
@@ -804,7 +802,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>154</v>
       </c>
@@ -812,7 +810,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>156</v>
       </c>
@@ -820,7 +818,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>158</v>
       </c>
@@ -828,7 +826,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>160</v>
       </c>

</xml_diff>